<commit_message>
increased size of example dataset
</commit_message>
<xml_diff>
--- a/data/rdcomponents_data.xlsx
+++ b/data/rdcomponents_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidcruvolo/Github/projects-rd-dashboards/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D89C3BED-7B6C-5C4C-9EAF-7517941F589F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF5FCC7E-FCE7-A54A-AFE9-94DDCC845B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-34640" yWindow="420" windowWidth="29400" windowHeight="17500" activeTab="2" xr2:uid="{F15013C8-4BA6-5F4B-9246-2FCF80075E48}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="37">
   <si>
     <t>name</t>
   </si>
@@ -143,6 +143,12 @@
   </si>
   <si>
     <t>city</t>
+  </si>
+  <si>
+    <t>province</t>
+  </si>
+  <si>
+    <t>type</t>
   </si>
 </sst>
 </file>
@@ -599,10 +605,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EC89AF0-EEE1-5648-8640-5548F157EC0D}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -821,6 +827,28 @@
         <v>22</v>
       </c>
     </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>